<commit_message>
Added DNI to MiniJTAG connector
</commit_message>
<xml_diff>
--- a/N3_WiFi/N3_WIFI_BOM_13Dec16.xlsx
+++ b/N3_WiFi/N3_WIFI_BOM_13Dec16.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="220">
   <si>
     <t>Netduino 3 Wi-Fi  Revised: Wednesday, February 25, 2015</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>MINI JTAG CONN HEADER 10POS UNSHD VERT SMD</t>
+  </si>
+  <si>
+    <t>DO NOT PLACE</t>
   </si>
   <si>
     <t>J9</t>
@@ -686,7 +689,7 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="14"/>
@@ -714,7 +717,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -729,35 +732,35 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -774,7 +777,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -782,14 +785,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,10 +800,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -817,49 +820,49 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -882,8 +885,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -932,14 +935,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -1034,9 +1037,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1116,7 +1119,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1144,10 +1147,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1403,9 +1406,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1693,7 +1696,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1721,10 +1724,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2698,7 +2701,9 @@
       <c r="G32" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="H32" s="3"/>
+      <c r="H32" t="s" s="2">
+        <v>115</v>
+      </c>
     </row>
     <row r="33" ht="14.6" customHeight="1">
       <c r="A33" s="4">
@@ -2708,19 +2713,19 @@
         <v>1</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E33" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F33" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="G33" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="H33" s="3"/>
     </row>
@@ -2732,19 +2737,19 @@
         <v>3</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E34" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F34" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="G34" t="s" s="2">
         <v>122</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>121</v>
       </c>
       <c r="H34" s="3"/>
     </row>
@@ -2756,19 +2761,19 @@
         <v>1</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E35" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F35" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="G35" t="s" s="2">
         <v>126</v>
-      </c>
-      <c r="G35" t="s" s="2">
-        <v>125</v>
       </c>
       <c r="H35" s="3"/>
     </row>
@@ -2780,19 +2785,19 @@
         <v>1</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D36" t="s" s="2">
         <v>13</v>
       </c>
       <c r="E36" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H36" s="3"/>
     </row>
@@ -2804,19 +2809,19 @@
         <v>1</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D37" t="s" s="2">
         <v>13</v>
       </c>
       <c r="E37" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H37" s="3"/>
     </row>
@@ -2828,19 +2833,19 @@
         <v>1</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D38" t="s" s="2">
         <v>13</v>
       </c>
       <c r="E38" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H38" s="3"/>
     </row>
@@ -2852,19 +2857,19 @@
         <v>6</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E39" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F39" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="G39" t="s" s="2">
         <v>142</v>
-      </c>
-      <c r="G39" t="s" s="2">
-        <v>141</v>
       </c>
       <c r="H39" s="3"/>
     </row>
@@ -2876,19 +2881,19 @@
         <v>1</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E40" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F40" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="G40" t="s" s="2">
         <v>145</v>
-      </c>
-      <c r="G40" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="H40" s="3"/>
     </row>
@@ -2900,19 +2905,19 @@
         <v>5</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E41" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F41" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="G41" t="s" s="2">
         <v>148</v>
-      </c>
-      <c r="G41" t="s" s="2">
-        <v>147</v>
       </c>
       <c r="H41" s="3"/>
     </row>
@@ -2924,19 +2929,19 @@
         <v>1</v>
       </c>
       <c r="C42" t="s" s="6">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D42" t="s" s="6">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E42" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F42" t="s" s="6">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G42" t="s" s="6">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H42" s="7"/>
     </row>
@@ -2948,22 +2953,22 @@
         <v>1</v>
       </c>
       <c r="C43" t="s" s="10">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D43" t="s" s="10">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E43" t="s" s="17">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F43" t="s" s="10">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G43" t="s" s="10">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H43" t="s" s="13">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" ht="14.6" customHeight="1">
@@ -2974,19 +2979,19 @@
         <v>5</v>
       </c>
       <c r="C44" t="s" s="15">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s" s="15">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E44" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F44" t="s" s="15">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G44" t="s" s="15">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H44" s="16"/>
     </row>
@@ -2998,19 +3003,19 @@
         <v>1</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E45" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H45" s="3"/>
     </row>
@@ -3022,16 +3027,16 @@
         <v>1</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D46" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E46" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G46" s="4">
         <v>390</v>
@@ -3046,19 +3051,19 @@
         <v>1</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E47" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H47" s="3"/>
     </row>
@@ -3070,16 +3075,16 @@
         <v>1</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G48" s="4">
         <v>22</v>
@@ -3094,19 +3099,19 @@
         <v>1</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E49" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H49" s="3"/>
     </row>
@@ -3118,19 +3123,19 @@
         <v>1</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E50" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H50" s="3"/>
     </row>
@@ -3142,16 +3147,16 @@
         <v>1</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E51" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G51" s="4">
         <v>680</v>
@@ -3166,19 +3171,19 @@
         <v>1</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D52" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E52" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H52" s="3"/>
     </row>
@@ -3190,19 +3195,19 @@
         <v>1</v>
       </c>
       <c r="C53" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D53" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E53" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H53" s="3"/>
     </row>
@@ -3214,19 +3219,19 @@
         <v>1</v>
       </c>
       <c r="C54" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D54" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E54" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F54" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="G54" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>195</v>
       </c>
       <c r="H54" s="3"/>
     </row>
@@ -3238,19 +3243,19 @@
         <v>1</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D55" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E55" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F55" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="G55" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="G55" t="s" s="2">
-        <v>199</v>
       </c>
       <c r="H55" s="3"/>
     </row>
@@ -3262,19 +3267,19 @@
         <v>1</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D56" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E56" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F56" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="G56" t="s" s="2">
         <v>203</v>
-      </c>
-      <c r="G56" t="s" s="2">
-        <v>202</v>
       </c>
       <c r="H56" s="3"/>
     </row>
@@ -3286,19 +3291,19 @@
         <v>1</v>
       </c>
       <c r="C57" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D57" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E57" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F57" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="G57" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="G57" t="s" s="2">
-        <v>205</v>
       </c>
       <c r="H57" s="3"/>
     </row>
@@ -3310,19 +3315,19 @@
         <v>1</v>
       </c>
       <c r="C58" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D58" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E58" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F58" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="G58" t="s" s="2">
         <v>210</v>
-      </c>
-      <c r="G58" t="s" s="2">
-        <v>209</v>
       </c>
       <c r="H58" s="3"/>
     </row>
@@ -3334,19 +3339,19 @@
         <v>1</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D59" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E59" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F59" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="G59" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="G59" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="H59" s="3"/>
     </row>
@@ -3358,19 +3363,19 @@
         <v>1</v>
       </c>
       <c r="C60" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D60" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E60" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H60" s="3"/>
     </row>
@@ -3378,7 +3383,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>